<commit_message>
Add sequence to reports... still has a bug for more than 1 report
</commit_message>
<xml_diff>
--- a/Sandbox.OpenXML/DStarExport.xlsx
+++ b/Sandbox.OpenXML/DStarExport.xlsx
@@ -12,9 +12,9 @@
     <x:workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12710" tabRatio="500" activeTab="1"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Overview" sheetId="2" r:id="rId1"/>
-    <x:sheet name="Data Model" sheetId="3" r:id="rId2"/>
-    <x:sheet name="Results Report" sheetId="1" r:id="rId3"/>
+    <x:sheet name="Overview" sheetId="2" r:id="Sequence1_rId1"/>
+    <x:sheet name="Data Model" sheetId="3" r:id="Sequence1_rId2"/>
+    <x:sheet name="Results Report" sheetId="1" r:id="Sequence1_rId3"/>
   </x:sheets>
   <x:calcPr calcId="150000" calcOnSave="0"/>
   <x:extLst>

</xml_diff>

<commit_message>
Strip code for reveal export
</commit_message>
<xml_diff>
--- a/Sandbox.OpenXML/DStarExport.xlsx
+++ b/Sandbox.OpenXML/DStarExport.xlsx
@@ -1,27 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <x:workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josueg\Documents\Projects\Deloitte\STAR Modernization - Deloitte Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12710" tabRatio="500" activeTab="1"/>
-  </x:bookViews>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
   <x:sheets>
-    <x:sheet name="Overview" sheetId="2" r:id="Sequence1_rId1"/>
-    <x:sheet name="Data Model" sheetId="3" r:id="Sequence1_rId2"/>
-    <x:sheet name="Results Report" sheetId="1" r:id="Sequence1_rId3"/>
+    <x:sheet name="Overview" sheetId="1" r:id="Sequence1_rId1"/>
+    <x:sheet name="Data Model" sheetId="2" r:id="Sequence1_rId2"/>
+    <x:sheet name="Results Report" sheetId="3" r:id="Sequence1_rId3"/>
   </x:sheets>
-  <x:calcPr calcId="150000" calcOnSave="0"/>
-  <x:extLst>
-    <x:ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" Flags="2"/>
-    </x:ext>
-  </x:extLst>
 </x:workbook>
 </file>
 
@@ -2246,267 +2230,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:dimension ref="A1:J86"/>

</xml_diff>